<commit_message>
updated powerpoint and additional beetle measurements
</commit_message>
<xml_diff>
--- a/Tyler/RealSizeMeasurementsWithPenny.xlsx
+++ b/Tyler/RealSizeMeasurementsWithPenny.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>From rope2 video</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t xml:space="preserve">Horizontal Average: </t>
+  </si>
+  <si>
+    <t>Horizonal Average:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horizontal average: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical Average: </t>
   </si>
 </sst>
 </file>
@@ -156,7 +165,7 @@
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -175,6 +184,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -202,6 +225,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="8"/>
         </patternFill>
       </fill>
@@ -217,6 +254,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -538,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y39"/>
+  <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,11 +614,15 @@
     <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.85546875" customWidth="1"/>
     <col min="22" max="22" width="16.85546875" customWidth="1"/>
-    <col min="24" max="24" width="9.5703125" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" customWidth="1"/>
+    <col min="23" max="23" width="16" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" customWidth="1"/>
+    <col min="28" max="28" width="18.28515625" customWidth="1"/>
+    <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,11 +638,11 @@
       <c r="U1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2">
         <f>AVERAGE(B4:B39)</f>
         <v>74.433333333333337</v>
@@ -609,7 +664,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -649,9 +704,9 @@
       <c r="R3" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="5">
         <f>AVERAGEIF(Q4:Q39,"&lt; 45",P4:P39)</f>
-        <v>50.616666666666653</v>
+        <v>50.499999999999986</v>
       </c>
       <c r="U3" t="s">
         <v>1</v>
@@ -659,14 +714,34 @@
       <c r="V3" t="s">
         <v>2</v>
       </c>
+      <c r="W3" t="s">
+        <v>10</v>
+      </c>
       <c r="X3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="5">
+        <f>AVERAGEIF(W4:W39,"&lt;= 45",V4:V39)</f>
+        <v>13.512500000000001</v>
+      </c>
+      <c r="AA3" t="s">
         <v>1</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AB3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE3" t="e">
+        <f>AVERAGEIF(AC4:AC39,"&lt; =45 ",AB4:AB39)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>135</v>
       </c>
@@ -679,6 +754,10 @@
       <c r="D4">
         <v>46</v>
       </c>
+      <c r="E4">
+        <f>C2/B2</f>
+        <v>0.77000298552022683</v>
+      </c>
       <c r="F4">
         <v>1</v>
       </c>
@@ -698,14 +777,14 @@
         <v>12</v>
       </c>
       <c r="M4" s="5">
-        <f>AVERAGEIF(K4:K39,"&lt; 45",J4:J39)</f>
+        <f>AVERAGEIF(K4:K39,"&lt;= 45",J4:J39)</f>
         <v>15.183333333333334</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4">
-        <v>56.8</v>
+        <v>54.7</v>
       </c>
       <c r="Q4" s="3">
         <v>14.28</v>
@@ -713,12 +792,38 @@
       <c r="R4" t="s">
         <v>11</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="4">
         <f>AVERAGEIF(Q4:Q39,"&gt; 45 ", P4:P39)</f>
-        <v>52.333333333333329</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>52.277777777777771</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>13.3</v>
+      </c>
+      <c r="W4">
+        <v>12.99</v>
+      </c>
+      <c r="X4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y4" s="4">
+        <f>AVERAGEIF(W4:W39,"&gt; 45",V4:V39)</f>
+        <v>14.74375</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE4" t="e">
+        <f>AVERAGEIF(AC4:AC39,"&gt; 45",AB4:AB40)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>150</v>
       </c>
@@ -751,13 +856,23 @@
         <v>17.622222222222224</v>
       </c>
       <c r="P5">
-        <v>56.6</v>
+        <v>55.6</v>
       </c>
       <c r="Q5" s="3">
         <v>69.33</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S5">
+        <f>S3/S4</f>
+        <v>0.96599362380446319</v>
+      </c>
+      <c r="V5">
+        <v>13.6</v>
+      </c>
+      <c r="W5">
+        <v>72.900000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>165</v>
       </c>
@@ -785,6 +900,10 @@
       <c r="K6">
         <v>3.58</v>
       </c>
+      <c r="M6">
+        <f>M4/M5</f>
+        <v>0.86160151324085743</v>
+      </c>
       <c r="O6">
         <v>15</v>
       </c>
@@ -794,8 +913,17 @@
       <c r="Q6" s="3">
         <v>80.05</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>25</v>
+      </c>
+      <c r="V6">
+        <v>13.2</v>
+      </c>
+      <c r="W6">
+        <v>81.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>180</v>
       </c>
@@ -826,8 +954,14 @@
       <c r="Q7" s="3">
         <v>10.68</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V7">
+        <v>14.6</v>
+      </c>
+      <c r="W7">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>195</v>
       </c>
@@ -864,8 +998,17 @@
       <c r="Q8" s="3">
         <v>78.69</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>50</v>
+      </c>
+      <c r="V8">
+        <v>11.4</v>
+      </c>
+      <c r="W8">
+        <v>15.26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>210</v>
       </c>
@@ -896,8 +1039,14 @@
       <c r="Q9" s="3">
         <v>13.24</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V9">
+        <v>14.3</v>
+      </c>
+      <c r="W9">
+        <v>77.91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>225</v>
       </c>
@@ -934,8 +1083,17 @@
       <c r="Q10" s="3">
         <v>77.91</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>75</v>
+      </c>
+      <c r="V10">
+        <v>13.6</v>
+      </c>
+      <c r="W10">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>240</v>
       </c>
@@ -966,8 +1124,14 @@
       <c r="Q11" s="3">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V11">
+        <v>13.9</v>
+      </c>
+      <c r="W11">
+        <v>56.71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>255</v>
       </c>
@@ -1004,8 +1168,17 @@
       <c r="Q12" s="3">
         <v>85.24</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>100</v>
+      </c>
+      <c r="V12">
+        <v>15</v>
+      </c>
+      <c r="W12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>270</v>
       </c>
@@ -1036,8 +1209,14 @@
       <c r="Q13" s="3">
         <v>11.56</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V13">
+        <v>15</v>
+      </c>
+      <c r="W13">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>280</v>
       </c>
@@ -1074,8 +1253,17 @@
       <c r="Q14" s="3">
         <v>77.83</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>125</v>
+      </c>
+      <c r="V14">
+        <v>13</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>292</v>
       </c>
@@ -1106,8 +1294,14 @@
       <c r="Q15" s="3">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V15">
+        <v>16</v>
+      </c>
+      <c r="W15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>326</v>
       </c>
@@ -1144,8 +1338,17 @@
       <c r="Q16" s="3">
         <v>82.61</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>150</v>
+      </c>
+      <c r="V16">
+        <v>14</v>
+      </c>
+      <c r="W16">
+        <v>85.91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>382</v>
       </c>
@@ -1176,8 +1379,14 @@
       <c r="Q17" s="3">
         <v>3.18</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V17">
+        <v>12</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>396</v>
       </c>
@@ -1211,8 +1420,17 @@
       <c r="Q18" s="3">
         <v>39.369999999999997</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>175</v>
+      </c>
+      <c r="V18">
+        <v>13.2</v>
+      </c>
+      <c r="W18">
+        <v>81.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>410</v>
       </c>
@@ -1243,8 +1461,14 @@
       <c r="Q19" s="3">
         <v>83.29</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V19">
+        <v>11.7</v>
+      </c>
+      <c r="W19">
+        <v>19.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>425</v>
       </c>
@@ -1281,8 +1505,17 @@
       <c r="Q20" s="3">
         <v>34.700000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>200</v>
+      </c>
+      <c r="V20">
+        <v>14.3</v>
+      </c>
+      <c r="W20">
+        <v>77.91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>440</v>
       </c>
@@ -1313,8 +1546,14 @@
       <c r="Q21" s="3">
         <v>73.61</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V21">
+        <v>13.3</v>
+      </c>
+      <c r="W21">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>455</v>
       </c>
@@ -1351,8 +1590,17 @@
       <c r="Q22" s="3">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U22">
+        <v>225</v>
+      </c>
+      <c r="V22">
+        <v>14</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>470</v>
       </c>
@@ -1383,8 +1631,14 @@
       <c r="Q23" s="3">
         <v>86.76</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V23">
+        <v>14.1</v>
+      </c>
+      <c r="W23">
+        <v>81.87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>485</v>
       </c>
@@ -1421,8 +1675,17 @@
       <c r="Q24" s="3">
         <v>83.02</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <v>250</v>
+      </c>
+      <c r="V24">
+        <v>13.9</v>
+      </c>
+      <c r="W24">
+        <v>59.74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>500</v>
       </c>
@@ -1453,8 +1716,14 @@
       <c r="Q25" s="3">
         <v>16.59</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V25">
+        <v>14</v>
+      </c>
+      <c r="W25">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>515</v>
       </c>
@@ -1491,8 +1760,17 @@
       <c r="Q26" s="3">
         <v>86.88</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U26">
+        <v>275</v>
+      </c>
+      <c r="V26">
+        <v>17</v>
+      </c>
+      <c r="W26">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>530</v>
       </c>
@@ -1523,8 +1801,14 @@
       <c r="Q27" s="3">
         <v>18.82</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V27">
+        <v>12</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>545</v>
       </c>
@@ -1561,8 +1845,17 @@
       <c r="Q28" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>300</v>
+      </c>
+      <c r="V28">
+        <v>17</v>
+      </c>
+      <c r="W28">
+        <v>86.63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>560</v>
       </c>
@@ -1593,8 +1886,14 @@
       <c r="Q29" s="3">
         <v>27.55</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V29">
+        <v>13</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>575</v>
       </c>
@@ -1631,8 +1930,17 @@
       <c r="Q30" s="3">
         <v>82.18</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U30">
+        <v>325</v>
+      </c>
+      <c r="V30">
+        <v>13.9</v>
+      </c>
+      <c r="W30">
+        <v>68.959999999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>590</v>
       </c>
@@ -1663,8 +1971,14 @@
       <c r="Q31" s="3">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V31">
+        <v>14</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>605</v>
       </c>
@@ -1701,8 +2015,17 @@
       <c r="Q32" s="3">
         <v>88.92</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U32">
+        <v>350</v>
+      </c>
+      <c r="V32">
+        <v>18.2</v>
+      </c>
+      <c r="W32">
+        <v>80.540000000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>620</v>
       </c>
@@ -1733,8 +2056,14 @@
       <c r="Q33" s="3">
         <v>31.33</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V33">
+        <v>17</v>
+      </c>
+      <c r="W33">
+        <v>28.07</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>635</v>
       </c>
@@ -1771,8 +2100,17 @@
       <c r="Q34" s="3">
         <v>76.760000000000005</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U34">
+        <v>375</v>
+      </c>
+      <c r="V34">
+        <v>14.3</v>
+      </c>
+      <c r="W34">
+        <v>24.78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>650</v>
       </c>
@@ -1803,8 +2141,14 @@
       <c r="Q35" s="3">
         <v>10.41</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V35">
+        <v>14.3</v>
+      </c>
+      <c r="W35">
+        <v>77.91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>665</v>
       </c>
@@ -1841,8 +2185,11 @@
       <c r="Q36" s="3">
         <v>88.78</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U36">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>680</v>
       </c>
@@ -1874,7 +2221,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>695</v>
       </c>
@@ -1912,7 +2259,7 @@
         <v>65.92</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>710</v>
       </c>
@@ -1946,13 +2293,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K4:M13 K14:K39">
-    <cfRule type="aboveAverage" dxfId="8" priority="5"/>
+    <cfRule type="aboveAverage" dxfId="12" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K39">
-    <cfRule type="aboveAverage" dxfId="7" priority="3" aboveAverage="0"/>
-    <cfRule type="aboveAverage" dxfId="6" priority="4" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="11" priority="5" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="10" priority="6" aboveAverage="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4:Q39">
+    <cfRule type="aboveAverage" dxfId="9" priority="3" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="8" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W4:W39">
     <cfRule type="aboveAverage" dxfId="0" priority="2"/>
     <cfRule type="aboveAverage" dxfId="1" priority="1" aboveAverage="0"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated model and measurement spreadsheet
</commit_message>
<xml_diff>
--- a/Tyler/RealSizeMeasurementsWithPenny.xlsx
+++ b/Tyler/RealSizeMeasurementsWithPenny.xlsx
@@ -165,14 +165,7 @@
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -184,62 +177,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
         </patternFill>
       </fill>
     </dxf>
@@ -591,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +596,10 @@
         <f>AVERAGE(G4:G39)</f>
         <v>12.616666666666667</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2">
+        <f>AVERAGE(J4:J39)</f>
+        <v>16.402777777777786</v>
+      </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -736,9 +676,9 @@
       <c r="AD3" t="s">
         <v>14</v>
       </c>
-      <c r="AE3" t="e">
-        <f>AVERAGEIF(AC4:AC39,"&lt; =45 ",AB4:AB39)</f>
-        <v>#DIV/0!</v>
+      <c r="AE3">
+        <f>AVERAGEIF(AC4:AC39,"&lt;= 45",AB4:AB39)</f>
+        <v>9.0333333333333332</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -815,12 +755,18 @@
       <c r="AA4">
         <v>1</v>
       </c>
+      <c r="AB4">
+        <v>12.2</v>
+      </c>
+      <c r="AC4">
+        <v>80.540000000000006</v>
+      </c>
       <c r="AD4" t="s">
         <v>11</v>
       </c>
-      <c r="AE4" t="e">
+      <c r="AE4" s="2">
         <f>AVERAGEIF(AC4:AC39,"&gt; 45",AB4:AB40)</f>
-        <v>#DIV/0!</v>
+        <v>10.866666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -871,6 +817,16 @@
       <c r="W5">
         <v>72.900000000000006</v>
       </c>
+      <c r="Y5">
+        <f>Y3/Y4</f>
+        <v>0.91649003815175922</v>
+      </c>
+      <c r="AB5">
+        <v>9</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -922,6 +878,15 @@
       <c r="W6">
         <v>81.25</v>
       </c>
+      <c r="AA6">
+        <v>25</v>
+      </c>
+      <c r="AB6">
+        <v>11.7</v>
+      </c>
+      <c r="AC6">
+        <v>59.04</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -960,6 +925,12 @@
       <c r="W7">
         <v>15.95</v>
       </c>
+      <c r="AB7">
+        <v>9.1</v>
+      </c>
+      <c r="AC7">
+        <v>6.34</v>
+      </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1007,6 +978,15 @@
       <c r="W8">
         <v>15.26</v>
       </c>
+      <c r="AA8">
+        <v>50</v>
+      </c>
+      <c r="AB8">
+        <v>11</v>
+      </c>
+      <c r="AC8">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1045,6 +1025,12 @@
       <c r="W9">
         <v>77.91</v>
       </c>
+      <c r="AB9">
+        <v>9.1</v>
+      </c>
+      <c r="AC9">
+        <v>6.34</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1092,6 +1078,15 @@
       <c r="W10">
         <v>17.100000000000001</v>
       </c>
+      <c r="AA10">
+        <v>75</v>
+      </c>
+      <c r="AB10">
+        <v>9.1</v>
+      </c>
+      <c r="AC10">
+        <v>83.66</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1130,6 +1125,12 @@
       <c r="W11">
         <v>56.71</v>
       </c>
+      <c r="AB11">
+        <v>10.4</v>
+      </c>
+      <c r="AC11">
+        <v>16.7</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1177,6 +1178,15 @@
       <c r="W12">
         <v>90</v>
       </c>
+      <c r="AA12">
+        <v>100</v>
+      </c>
+      <c r="AB12">
+        <v>8.5</v>
+      </c>
+      <c r="AC12">
+        <v>20.56</v>
+      </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1215,6 +1225,12 @@
       <c r="W13">
         <v>3.81</v>
       </c>
+      <c r="AB13">
+        <v>11.2</v>
+      </c>
+      <c r="AC13">
+        <v>79.7</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1262,6 +1278,15 @@
       <c r="W14">
         <v>0</v>
       </c>
+      <c r="AA14">
+        <v>125</v>
+      </c>
+      <c r="AB14">
+        <v>10</v>
+      </c>
+      <c r="AC14">
+        <v>84.29</v>
+      </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1300,6 +1325,12 @@
       <c r="W15">
         <v>90</v>
       </c>
+      <c r="AB15">
+        <v>8.1</v>
+      </c>
+      <c r="AC15">
+        <v>7.13</v>
+      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1347,6 +1378,9 @@
       <c r="W16">
         <v>85.91</v>
       </c>
+      <c r="AA16">
+        <v>150</v>
+      </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -2293,19 +2327,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K4:M13 K14:K39">
-    <cfRule type="aboveAverage" dxfId="12" priority="7"/>
+    <cfRule type="aboveAverage" dxfId="8" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K39">
-    <cfRule type="aboveAverage" dxfId="11" priority="5" aboveAverage="0"/>
-    <cfRule type="aboveAverage" dxfId="10" priority="6" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="7" priority="7" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="6" priority="8" aboveAverage="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4:Q39">
-    <cfRule type="aboveAverage" dxfId="9" priority="3" aboveAverage="0"/>
-    <cfRule type="aboveAverage" dxfId="8" priority="4"/>
+    <cfRule type="aboveAverage" dxfId="5" priority="5" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="4" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4:W39">
-    <cfRule type="aboveAverage" dxfId="0" priority="2"/>
-    <cfRule type="aboveAverage" dxfId="1" priority="1" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="3" priority="4"/>
+    <cfRule type="aboveAverage" dxfId="2" priority="3" aboveAverage="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC4:AC38">
+    <cfRule type="aboveAverage" dxfId="1" priority="2"/>
+    <cfRule type="aboveAverage" dxfId="0" priority="1" aboveAverage="0"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>